<commit_message>
Add Turn Off Command for admin
</commit_message>
<xml_diff>
--- a/STR.xlsx
+++ b/STR.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="304">
   <si>
     <t>Variable (NO EDIT)</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Broadcast Message (All Users)</t>
+  </si>
+  <si>
+    <t>admin_mm_btn_5</t>
+  </si>
+  <si>
+    <t>TurnOff Bot</t>
   </si>
   <si>
     <t>confirm_action_ask</t>
@@ -711,16 +717,16 @@
     <t>price_eye</t>
   </si>
   <si>
-    <t xml:space="preserve">👁 Price: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">👁 قيمت: </t>
+    <t>👁 Price:</t>
+  </si>
+  <si>
+    <t>👁 قيمت:</t>
   </si>
   <si>
     <t>euros_per</t>
   </si>
   <si>
-    <t xml:space="preserve">euros per </t>
+    <t>euros per</t>
   </si>
   <si>
     <t>یورو</t>
@@ -1712,56 +1718,62 @@
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" ht="21.0" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" ht="21.0" customHeight="1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" ht="21.0" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" ht="21.0" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" ht="21.0" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" ht="21.0" customHeight="1">
       <c r="A19" s="5"/>
@@ -2073,20 +2085,20 @@
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
+    <row r="81" ht="21.0" customHeight="1">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+    </row>
+    <row r="82" ht="21.0" customHeight="1">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" ht="21.0" customHeight="1">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="7"/>
@@ -6697,6 +6709,21 @@
       <c r="A1005" s="7"/>
       <c r="B1005" s="7"/>
       <c r="C1005" s="7"/>
+    </row>
+    <row r="1006" ht="15.75" customHeight="1">
+      <c r="A1006" s="7"/>
+      <c r="B1006" s="7"/>
+      <c r="C1006" s="7"/>
+    </row>
+    <row r="1007" ht="15.75" customHeight="1">
+      <c r="A1007" s="7"/>
+      <c r="B1007" s="7"/>
+      <c r="C1007" s="7"/>
+    </row>
+    <row r="1008" ht="15.75" customHeight="1">
+      <c r="A1008" s="7"/>
+      <c r="B1008" s="7"/>
+      <c r="C1008" s="7"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -6736,13 +6763,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -6752,24 +6779,24 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
@@ -6784,24 +6811,24 @@
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -6811,24 +6838,24 @@
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="1">
@@ -6838,24 +6865,24 @@
     </row>
     <row r="14" ht="21.0" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="1">
@@ -6865,24 +6892,24 @@
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="21.0" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" ht="21.0" customHeight="1">
@@ -6892,13 +6919,13 @@
     </row>
     <row r="20" ht="21.0" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
@@ -7021,497 +7048,497 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" ht="21.0" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" ht="21.0" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" ht="21.0" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" ht="21.0" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" ht="21.0" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" ht="21.0" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" ht="21.0" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" ht="21.0" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" ht="21.0" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" ht="21.0" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" ht="21.0" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" ht="21.0" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" ht="21.0" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" ht="21.0" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" ht="21.0" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" ht="21.0" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" ht="21.0" customHeight="1">
       <c r="A36" s="13" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" ht="21.0" customHeight="1">
       <c r="A37" s="13" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" ht="21.0" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" ht="21.0" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" ht="21.0" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" ht="21.0" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" ht="21.0" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" ht="21.0" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" ht="21.0" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" ht="21.0" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" ht="21.0" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" ht="21.0" customHeight="1">
@@ -7521,68 +7548,68 @@
     </row>
     <row r="48" ht="21.0" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" ht="21.0" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" ht="21.0" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" ht="21.0" customHeight="1">
       <c r="A51" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" ht="21.0" customHeight="1">
       <c r="A52" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" ht="21.0" customHeight="1">
       <c r="A53" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" ht="21.0" customHeight="1">
@@ -7592,46 +7619,46 @@
     </row>
     <row r="55" ht="21.0" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" ht="21.0" customHeight="1">
       <c r="A56" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="C56" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" ht="21.0" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" ht="21.0" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -7671,35 +7698,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -7709,46 +7736,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -7938,46 +7965,46 @@
     </row>
     <row r="47" ht="21.0" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" ht="21.0" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" ht="21.0" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" ht="21.0" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" ht="21.0" customHeight="1">
@@ -8022,35 +8049,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -8060,46 +8087,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -8339,35 +8366,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -8377,46 +8404,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>260</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -8654,123 +8681,123 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>292</v>
-      </c>
       <c r="C12" s="16" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="1">
@@ -10013,35 +10040,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">

</xml_diff>

<commit_message>
Add categories + expired ad
</commit_message>
<xml_diff>
--- a/STR.xlsx
+++ b/STR.xlsx
@@ -16,6 +16,8 @@
     <sheet state="visible" name="selling_goods" sheetId="11" r:id="rId14"/>
     <sheet state="visible" name="buying_goods" sheetId="12" r:id="rId15"/>
     <sheet state="visible" name="buying_cargo" sheetId="13" r:id="rId16"/>
+    <sheet state="visible" name="selling_cargo" sheetId="14" r:id="rId17"/>
+    <sheet state="visible" name="buying_euro" sheetId="15" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="523">
   <si>
     <t>Variable (NO EDIT)</t>
   </si>
@@ -968,7 +970,13 @@
     <t>آگهی در حال ساخت شما حذف شد ✅</t>
   </si>
   <si>
-    <t>error3</t>
+    <t>ad_expired</t>
+  </si>
+  <si>
+    <t>Your Ad Expired</t>
+  </si>
+  <si>
+    <t>ad_delete_error</t>
   </si>
   <si>
     <t>Your Ad can't be deleted</t>
@@ -977,6 +985,18 @@
     <t>حذف آگهی شما امکان پذیر نمی باشد ❌</t>
   </si>
   <si>
+    <t>ad_expired_error</t>
+  </si>
+  <si>
+    <t>Your Ad can't be expired</t>
+  </si>
+  <si>
+    <t>ad_expired_line</t>
+  </si>
+  <si>
+    <t>🆘️️❌️️ This ad has expired❌️️🆘️️</t>
+  </si>
+  <si>
     <t>rent_confirm_delete_ad</t>
   </si>
   <si>
@@ -984,6 +1004,12 @@
   </si>
   <si>
     <t>تایید حذف آگهی؟</t>
+  </si>
+  <si>
+    <t>rent_confirm_expire_ad</t>
+  </si>
+  <si>
+    <t>Confirm Expire Ad?</t>
   </si>
   <si>
     <t>rent_hint_text_confirm_or_cancel</t>
@@ -1200,6 +1226,9 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
+    <t>error3</t>
+  </si>
+  <si>
     <t>home_applicant_btn</t>
   </si>
   <si>
@@ -1817,66 +1846,277 @@
   </si>
   <si>
     <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍 related to the city: #[city]
-🔎 Area: [sub_city]
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
 [description]</t>
   </si>
   <si>
+    <t>buying_cargo_user_view_ad</t>
+  </si>
+  <si>
+    <t>buying_cargo_admin_preview</t>
+  </si>
+  <si>
     <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍مربوط به شهر:  #[city]
-🔎 محدوده: [sub_city]
-[description]</t>
-  </si>
-  <si>
-    <t>buying_cargo_user_view_ad</t>
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>buying_cargo_channel_message</t>
   </si>
   <si>
     <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍 related to the city: #[city]
-🔎 Area: [sub_city]
-[description]</t>
-  </si>
-  <si>
-    <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍مربوط به شهر:  #[city]
-🔎 محدوده: [sub_city]
-[description]</t>
-  </si>
-  <si>
-    <t>buying_cargo_admin_preview</t>
-  </si>
-  <si>
-    <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍 related to the city: #[city]
-🔎 Area: [sub_city]
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
 [description]
 Contact the [advertiser]
 🤖️️️ @bot_username
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍مربوط به شهر:  #[city]
-🔎 محدوده: [sub_city]
+    <t>selling_cargo_btn</t>
+  </si>
+  <si>
+    <t>selling Cargo</t>
+  </si>
+  <si>
+    <t>selling_cargo_t1</t>
+  </si>
+  <si>
+    <t>category: selling Cargo</t>
+  </si>
+  <si>
+    <t>selling_cargo_t2</t>
+  </si>
+  <si>
+    <t>selling_cargo_origin</t>
+  </si>
+  <si>
+    <t>selling_cargo_origin_label</t>
+  </si>
+  <si>
+    <t>selling_cargo_destination</t>
+  </si>
+  <si>
+    <t>selling_cargo_destination_label</t>
+  </si>
+  <si>
+    <t>selling_cargo_flight_date</t>
+  </si>
+  <si>
+    <t>selling_cargo_flight_date_label</t>
+  </si>
+  <si>
+    <t>selling_cargo_price</t>
+  </si>
+  <si>
+    <t>selling_cargo_price_label</t>
+  </si>
+  <si>
+    <t>selling_cargo_load</t>
+  </si>
+  <si>
+    <t>selling_cargo_load_label</t>
+  </si>
+  <si>
+    <t>selling_cargo_od_label</t>
+  </si>
+  <si>
+    <t>selling_cargo_ia_btn</t>
+  </si>
+  <si>
+    <t>selling_cargo_ai_btn</t>
+  </si>
+  <si>
+    <t>selling_cargo_ia</t>
+  </si>
+  <si>
+    <t>selling_cargo_ai</t>
+  </si>
+  <si>
+    <t>selling_cargo_iran</t>
+  </si>
+  <si>
+    <t>selling_cargo_austria</t>
+  </si>
+  <si>
+    <t>selling_cargo_user_preview</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ #selling_cargo ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]</t>
+  </si>
+  <si>
+    <t>selling_cargo_user_view_ad</t>
+  </si>
+  <si>
+    <t>selling_cargo_admin_preview</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ #selling_cargo ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
 [description]
-👤تماس با [advertiser]</t>
-  </si>
-  <si>
-    <t>buying_cargo_channel_message</t>
-  </si>
-  <si>
-    <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
-Product Name: [product_name]
-📍مربوط به شهر:  #[city]
-🔎 محدوده: [sub_city]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>selling_cargo_channel_message</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ #selling_cargo ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
 [description]
-👤تماس با [advertiser]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
+  <si>
+    <t>buying_euro_btn</t>
+  </si>
+  <si>
+    <t>euro sell</t>
+  </si>
+  <si>
+    <t>buying_euro_t1</t>
+  </si>
+  <si>
+    <t>category: euro sell</t>
+  </si>
+  <si>
+    <t>buying_euro_t2</t>
+  </si>
+  <si>
+    <t>how many euros do you want to sell</t>
+  </si>
+  <si>
+    <t>buying_euro_tomans</t>
+  </si>
+  <si>
+    <t>how many tomans do you want to sell each euro?</t>
+  </si>
+  <si>
+    <t>buying_euro_transfer</t>
+  </si>
+  <si>
+    <t>specify how to transfer euros:</t>
+  </si>
+  <si>
+    <t>specify how to transger euros:</t>
+  </si>
+  <si>
+    <t>euro_transfer_1</t>
+  </si>
+  <si>
+    <t>PayPal</t>
+  </si>
+  <si>
+    <t>euro_transfer_2</t>
+  </si>
+  <si>
+    <t>Revolut</t>
+  </si>
+  <si>
+    <t>euro_transfer_3</t>
+  </si>
+  <si>
+    <t>Monese</t>
+  </si>
+  <si>
+    <t>euro_transfer_4</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>euro_transfer_5</t>
+  </si>
+  <si>
+    <t>Wise</t>
+  </si>
+  <si>
+    <t>euro_transfer_6</t>
+  </si>
+  <si>
+    <t>arz digital</t>
+  </si>
+  <si>
+    <t>euro_transfer_7</t>
+  </si>
+  <si>
+    <t>by person</t>
+  </si>
+  <si>
+    <t>buying_euro_user_preview</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ #buying_euro ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]</t>
+  </si>
+  <si>
+    <t>buying_euro_user_view_ad</t>
+  </si>
+  <si>
+    <t>buying_euro_admin_preview</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ #buying_euro ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>buying_euro_channel_message</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ #buying_euro ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]
 🤖️️️ @bot_username
 ✅️️️️️️️ @channel_username</t>
   </si>
@@ -1952,7 +2192,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2005,6 +2245,9 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2032,6 +2275,14 @@
 </file>
 
 <file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3661,29 +3912,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -3699,46 +3950,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -3979,29 +4230,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -4017,46 +4268,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -4292,29 +4543,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -4330,46 +4581,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -4605,143 +4856,909 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>409</v>
-      </c>
+      <c r="A3" s="16"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>413</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" ht="21.0" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" ht="21.0" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="11" ht="21.0" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="12" ht="21.0" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" ht="21.0" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" ht="21.0" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="15" ht="21.0" customHeight="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" ht="21.0" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" ht="21.0" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="18" ht="21.0" customHeight="1">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" ht="21.0" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" ht="21.0" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" ht="21.0" customHeight="1">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" ht="21.0" customHeight="1">
+      <c r="A22" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="23" ht="21.0" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" ht="21.0" customHeight="1">
+      <c r="A24" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="25" ht="21.0" customHeight="1">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" ht="21.0" customHeight="1">
+      <c r="A26" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="27" ht="21.0" customHeight="1">
+      <c r="A27" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28" ht="21.0" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="29" ht="21.0" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="30" ht="21.0" customHeight="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" ht="21.0" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32" ht="21.0" customHeight="1">
+      <c r="A32" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="33" ht="21.0" customHeight="1">
+      <c r="A33" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="34" ht="21.0" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" ht="21.0" customHeight="1">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" ht="21.0" customHeight="1">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="11"/>
+    </row>
+    <row r="37" ht="21.0" customHeight="1">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="11"/>
+    </row>
+    <row r="38" ht="21.0" customHeight="1">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="11"/>
+    </row>
+    <row r="39" ht="21.0" customHeight="1">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" ht="21.0" customHeight="1">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" ht="21.0" customHeight="1">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FF011627"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.5"/>
+    <col customWidth="1" min="2" max="2" width="38.38"/>
+    <col customWidth="1" min="3" max="3" width="38.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="21.0" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="21.0" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3" ht="21.0" customHeight="1">
+      <c r="A3" s="16"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" ht="21.0" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" ht="21.0" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" ht="21.0" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" ht="21.0" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" ht="21.0" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" ht="21.0" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" ht="21.0" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="11" ht="21.0" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="12" ht="21.0" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" ht="21.0" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" ht="21.0" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="15" ht="21.0" customHeight="1">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" ht="21.0" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" ht="21.0" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="18" ht="21.0" customHeight="1">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" ht="21.0" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="20" ht="21.0" customHeight="1">
+      <c r="A20" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" ht="21.0" customHeight="1">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" ht="21.0" customHeight="1">
+      <c r="A22" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="23" ht="21.0" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" ht="21.0" customHeight="1">
+      <c r="A24" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="25" ht="21.0" customHeight="1">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" ht="21.0" customHeight="1">
+      <c r="A26" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="27" ht="21.0" customHeight="1">
+      <c r="A27" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28" ht="21.0" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="29" ht="21.0" customHeight="1">
+      <c r="A29" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="30" ht="21.0" customHeight="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" ht="21.0" customHeight="1">
+      <c r="A31" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="32" ht="21.0" customHeight="1">
+      <c r="A32" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="33" ht="21.0" customHeight="1">
+      <c r="A33" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="34" ht="21.0" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="35" ht="21.0" customHeight="1">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" ht="21.0" customHeight="1">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="11"/>
+    </row>
+    <row r="37" ht="21.0" customHeight="1">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="11"/>
+    </row>
+    <row r="38" ht="21.0" customHeight="1">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="11"/>
+    </row>
+    <row r="39" ht="21.0" customHeight="1">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="11"/>
+    </row>
+    <row r="40" ht="21.0" customHeight="1">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" ht="21.0" customHeight="1">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <tabColor rgb="FF011627"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.5"/>
+    <col customWidth="1" min="2" max="2" width="38.38"/>
+    <col customWidth="1" min="3" max="3" width="38.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="21.0" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="21.0" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="3" ht="21.0" customHeight="1">
+      <c r="A3" s="16"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" ht="21.0" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5" ht="21.0" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" ht="21.0" customHeight="1">
+      <c r="A6" s="16"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" ht="21.0" customHeight="1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" ht="21.0" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>416</v>
+        <v>499</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>417</v>
+        <v>500</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>417</v>
+        <v>501</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>418</v>
+        <v>502</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>419</v>
+        <v>503</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>417</v>
+        <v>503</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>420</v>
+        <v>506</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>421</v>
+        <v>507</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>421</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>422</v>
+        <v>508</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>423</v>
+        <v>509</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>423</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>424</v>
+        <v>512</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>425</v>
+        <v>513</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>425</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>426</v>
+        <v>514</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>427</v>
+        <v>515</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>427</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
@@ -4750,352 +5767,53 @@
       <c r="C17" s="7"/>
     </row>
     <row r="18" ht="21.0" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>429</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" ht="21.0" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>430</v>
+        <v>516</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>431</v>
+        <v>517</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>431</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" ht="21.0" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>432</v>
+        <v>519</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>433</v>
+        <v>520</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>433</v>
+        <v>520</v>
       </c>
     </row>
     <row r="22" ht="21.0" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>434</v>
+        <v>521</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>435</v>
+        <v>522</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="23" ht="21.0" customHeight="1">
-      <c r="A23" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="24" ht="21.0" customHeight="1">
-      <c r="A24" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>439</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="25" ht="21.0" customHeight="1">
-      <c r="A25" s="16" t="s">
-        <v>440</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>441</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="26" ht="21.0" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>443</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="27" ht="21.0" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="28" ht="21.0" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" ht="21.0" customHeight="1">
-      <c r="A29" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="30" ht="21.0" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>449</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="31" ht="21.0" customHeight="1">
-      <c r="A31" s="7" t="s">
-        <v>452</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="32" ht="21.0" customHeight="1">
-      <c r="A32" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="33" ht="21.0" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" ht="21.0" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" ht="21.0" customHeight="1">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" ht="21.0" customHeight="1">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" ht="21.0" customHeight="1">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" ht="21.0" customHeight="1">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" ht="21.0" customHeight="1">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" ht="21.0" customHeight="1">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="11"/>
-    </row>
-    <row r="41" ht="21.0" customHeight="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" ht="21.0" customHeight="1">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" ht="21.0" customHeight="1">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="11"/>
-    </row>
-    <row r="44" ht="21.0" customHeight="1">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="11"/>
-    </row>
-    <row r="45" ht="21.0" customHeight="1">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="11"/>
-    </row>
-    <row r="46" ht="21.0" customHeight="1">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="11"/>
-    </row>
-    <row r="47" ht="21.0" customHeight="1">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="11"/>
-    </row>
-    <row r="48" ht="21.0" customHeight="1">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="11"/>
-    </row>
-    <row r="49" ht="21.0" customHeight="1">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="11"/>
-    </row>
-    <row r="50" ht="21.0" customHeight="1">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="11"/>
-    </row>
-    <row r="51" ht="21.0" customHeight="1">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="11"/>
-    </row>
-    <row r="52" ht="21.0" customHeight="1">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="11"/>
-    </row>
-    <row r="53" ht="21.0" customHeight="1">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" ht="21.0" customHeight="1">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="11"/>
-    </row>
-    <row r="55" ht="21.0" customHeight="1">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="11"/>
-    </row>
-    <row r="56" ht="21.0" customHeight="1">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="11"/>
-    </row>
-    <row r="57" ht="21.0" customHeight="1">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="11"/>
-    </row>
-    <row r="58" ht="21.0" customHeight="1">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="11"/>
-    </row>
-    <row r="59" ht="21.0" customHeight="1">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="11"/>
-    </row>
-    <row r="60" ht="21.0" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="11"/>
-    </row>
-    <row r="61" ht="21.0" customHeight="1">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="11"/>
-    </row>
-    <row r="62" ht="21.0" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="11"/>
-    </row>
-    <row r="63" ht="21.0" customHeight="1">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="11"/>
-    </row>
-    <row r="64" ht="21.0" customHeight="1">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="11"/>
-    </row>
-    <row r="65" ht="21.0" customHeight="1">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="11"/>
-    </row>
-    <row r="66" ht="21.0" customHeight="1">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="11"/>
-    </row>
-    <row r="67" ht="21.0" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="11"/>
-    </row>
-    <row r="68" ht="21.0" customHeight="1">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="11"/>
-    </row>
-    <row r="69" ht="21.0" customHeight="1">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="11"/>
-    </row>
-    <row r="70" ht="21.0" customHeight="1">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="11"/>
-    </row>
-    <row r="71" ht="21.0" customHeight="1">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="14"/>
+        <v>522</v>
+      </c>
     </row>
   </sheetData>
   <printOptions/>
@@ -11923,910 +12641,914 @@
       <c r="C4" s="11"/>
     </row>
     <row r="5" ht="21.0" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="11"/>
+      <c r="A6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="11"/>
+      <c r="A10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>98</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" ht="21.0" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>101</v>
+        <v>115</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>104</v>
+        <v>117</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>107</v>
+        <v>119</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>110</v>
+        <v>121</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" ht="21.0" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>113</v>
+        <v>123</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" ht="21.0" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="20" ht="21.0" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" ht="21.0" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" ht="21.0" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" ht="21.0" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" ht="21.0" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" ht="21.0" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" ht="21.0" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" ht="21.0" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" ht="21.0" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" ht="21.0" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" ht="21.0" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" ht="21.0" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" ht="21.0" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" ht="21.0" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" ht="21.0" customHeight="1">
-      <c r="A36" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>147</v>
-      </c>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" ht="21.0" customHeight="1">
       <c r="A37" s="7" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>149</v>
+        <v>159</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="38" ht="21.0" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>151</v>
+        <v>162</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="39" ht="21.0" customHeight="1">
-      <c r="A39" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>153</v>
-      </c>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="11"/>
     </row>
     <row r="40" ht="21.0" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>155</v>
+        <v>165</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="41" ht="21.0" customHeight="1">
       <c r="A41" s="7" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>157</v>
+        <v>168</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="42" ht="21.0" customHeight="1">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="11"/>
+      <c r="A42" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="43" ht="21.0" customHeight="1">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="11"/>
+      <c r="A43" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="44" ht="21.0" customHeight="1">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="11"/>
+      <c r="A44" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="45" ht="21.0" customHeight="1">
       <c r="A45" s="7" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" ht="21.0" customHeight="1">
       <c r="A46" s="7" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" ht="21.0" customHeight="1">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="11"/>
+      <c r="A47" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="48" ht="21.0" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" ht="21.0" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" ht="21.0" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" ht="21.0" customHeight="1">
       <c r="A51" s="7" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" ht="21.0" customHeight="1">
       <c r="A52" s="7" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" ht="21.0" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" ht="21.0" customHeight="1">
       <c r="A54" s="7" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" ht="21.0" customHeight="1">
       <c r="A55" s="7" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" ht="21.0" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" ht="21.0" customHeight="1">
       <c r="A57" s="7" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" ht="21.0" customHeight="1">
       <c r="A58" s="7" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" ht="21.0" customHeight="1">
       <c r="A59" s="7" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" ht="21.0" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" ht="21.0" customHeight="1">
       <c r="A61" s="7" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" ht="21.0" customHeight="1">
       <c r="A62" s="7" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" ht="21.0" customHeight="1">
-      <c r="A63" s="7" t="s">
-        <v>209</v>
+      <c r="A63" s="16" t="s">
+        <v>233</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" ht="21.0" customHeight="1">
-      <c r="A64" s="7" t="s">
-        <v>212</v>
+      <c r="A64" s="16" t="s">
+        <v>236</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" ht="21.0" customHeight="1">
       <c r="A65" s="7" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" ht="21.0" customHeight="1">
       <c r="A66" s="7" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" ht="21.0" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
     </row>
     <row r="68" ht="21.0" customHeight="1">
       <c r="A68" s="7" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" ht="21.0" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" ht="21.0" customHeight="1">
       <c r="A70" s="7" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
     </row>
     <row r="71" ht="21.0" customHeight="1">
-      <c r="A71" s="16" t="s">
-        <v>233</v>
+      <c r="A71" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" ht="21.0" customHeight="1">
-      <c r="A72" s="16" t="s">
-        <v>236</v>
+      <c r="A72" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" ht="21.0" customHeight="1">
       <c r="A73" s="7" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" ht="21.0" customHeight="1">
       <c r="A74" s="7" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>244</v>
+        <v>267</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="75" ht="21.0" customHeight="1">
       <c r="A75" s="7" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" ht="21.0" customHeight="1">
       <c r="A76" s="7" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>250</v>
+        <v>272</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="77" ht="21.0" customHeight="1">
       <c r="A77" s="7" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
     </row>
     <row r="78" ht="21.0" customHeight="1">
       <c r="A78" s="7" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>256</v>
+        <v>277</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="79" ht="21.0" customHeight="1">
       <c r="A79" s="7" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>259</v>
+        <v>279</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="80" ht="21.0" customHeight="1">
       <c r="A80" s="7" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
     </row>
     <row r="81" ht="21.0" customHeight="1">
-      <c r="A81" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>265</v>
+      <c r="A81" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="82" ht="21.0" customHeight="1">
       <c r="A82" s="7" t="s">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>267</v>
+        <v>286</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="83" ht="21.0" customHeight="1">
       <c r="A83" s="7" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="84" ht="21.0" customHeight="1">
       <c r="A84" s="7" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="85" ht="21.0" customHeight="1">
-      <c r="A85" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>276</v>
-      </c>
+      <c r="A85" s="13"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="14"/>
     </row>
     <row r="86" ht="21.0" customHeight="1">
       <c r="A86" s="7" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87" ht="21.0" customHeight="1">
       <c r="A87" s="7" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
     </row>
     <row r="88" ht="21.0" customHeight="1">
       <c r="A88" s="7" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89" ht="21.0" customHeight="1">
-      <c r="A89" s="13"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="14"/>
-    </row>
-    <row r="90" ht="21.0" customHeight="1">
-      <c r="A90" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="91" ht="21.0" customHeight="1">
-      <c r="A91" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="92" ht="21.0" customHeight="1">
-      <c r="A92" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="93" ht="21.0" customHeight="1">
-      <c r="A93" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>295</v>
+      <c r="A89" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -12867,29 +13589,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>298</v>
+        <v>304</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -12905,46 +13627,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -13145,35 +13867,35 @@
     </row>
     <row r="48" ht="21.0" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>271</v>
+        <v>323</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" ht="21.0" customHeight="1">
       <c r="A49" s="7" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" ht="21.0" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="51" ht="21.0" customHeight="1">
@@ -13219,29 +13941,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>316</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>316</v>
+        <v>324</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -13257,46 +13979,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -13537,29 +14259,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -13575,46 +14297,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -13855,29 +14577,29 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>94</v>
@@ -13893,46 +14615,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">

</xml_diff>

<commit_message>
Fix description and reorder main menu items
</commit_message>
<xml_diff>
--- a/STR.xlsx
+++ b/STR.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="656">
   <si>
     <t>Variable (NO EDIT)</t>
   </si>
@@ -136,7 +136,7 @@
     <t>CANCEL</t>
   </si>
   <si>
-    <t>لغو آگهی ❌</t>
+    <t>لغو ❌</t>
   </si>
   <si>
     <t>canceled_t</t>
@@ -154,7 +154,7 @@
     <t>CONFIRM</t>
   </si>
   <si>
-    <t>ارسال آگهی ✅</t>
+    <t>تایید ✅</t>
   </si>
   <si>
     <t>confirmed_t</t>
@@ -205,58 +205,24 @@
     <t>english</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t xml:space="preserve">✅ ثبت آگهی در کانال @austriabazar فقط توسط این ربات و پس از تایید ادمین صورت می گیرد.
+    <t xml:space="preserve">✅ ثبت آگهی در کانال @AustriaBazar فقط توسط این ربات و پس از تایید ادمین صورت می گیرد.
 ✅ نیازی به نوشتن ID در آگهی نمی باشد.
 ✅ ارسال انواع آگهی مجاز است.
 ✅ می توانید پس از ثبت یک آگهی و قبل از تایید یا رد آگهی توسط ادمین، شروع به ثبت آگهی های بعدی خود نمایید.
 ⚠️ صحت آگهی بر عهده آگهی دهنده است و AustriaBazar هیچ گونه مسئولیتی در قبال آگهی قبول نمی کند.
 کانال های ما : 
 @AustriaBazar
-@AustriaEverything
 گروه ما:
 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="12.0"/>
-        <u/>
-      </rPr>
-      <t>https://t.me/Austria_Everything</t>
-    </r>
   </si>
   <si>
     <t>short_description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t xml:space="preserve">ربات ثبت آگهی در کانال @AustriaBazar
+    <t xml:space="preserve">ربات ثبت آگهی در کانال @AustriaBazar
 کانال ما:
-@AustriaEverything
 گروه ما:
 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="12.0"/>
-        <u/>
-      </rPr>
-      <t>https://t.me/Austria_Everything</t>
-    </r>
   </si>
   <si>
     <t>mm_m</t>
@@ -402,7 +368,7 @@
     <t>Rent</t>
   </si>
   <si>
-    <t>اجاره خانه🏠</t>
+    <t>اجاره خانه 🏠</t>
   </si>
   <si>
     <t>rent_t1</t>
@@ -411,7 +377,7 @@
     <t>category: rent</t>
   </si>
   <si>
-    <t>📦 دسته بندی : اجاره خانه</t>
+    <t>📁 دسته بندی: اجاره خانه 🏠</t>
   </si>
   <si>
     <t>rent_t2</t>
@@ -1138,7 +1104,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_خانه ✅️️️️💠
+    <t>💠✅️️️️ #اجاره_خانه ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1163,7 +1129,7 @@
 Contact the [advertiser]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_خانه ✅️️️️💠
+    <t>💠✅️️️️ #اجاره_خانه ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1188,7 +1154,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_خانه ✅️️️️💠
+    <t>💠✅️️️️ #اجاره_خانه ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1206,7 +1172,7 @@
     <t>home applicant</t>
   </si>
   <si>
-    <t>متقاضی خانه🏠</t>
+    <t>متقاضی خانه 🏠</t>
   </si>
   <si>
     <t>home_applicant_t1</t>
@@ -1215,7 +1181,7 @@
     <t>category: home applicant</t>
   </si>
   <si>
-    <t>📦 دسته بندی : متقاضی خانه</t>
+    <t>📁 دسته بندی: متقاضی خانه 🏠</t>
   </si>
   <si>
     <t>home_applicant_t2</t>
@@ -1232,7 +1198,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره اتاق ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_خانه ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1264,7 +1230,7 @@
 Contact the [advertiser]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره اتاق ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_خانه ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1287,7 +1253,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره اتاق ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_خانه ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1304,7 +1270,7 @@
     <t>room rent</t>
   </si>
   <si>
-    <t>اجاره اتاق🏠</t>
+    <t>اجاره اتاق 🚪🛏️</t>
   </si>
   <si>
     <t>room_rent_t1</t>
@@ -1313,13 +1279,10 @@
     <t>category: room rent</t>
   </si>
   <si>
-    <t>📦 دسته بندی : اجاره اتاق</t>
+    <t>📁 دسته بندی: اجاره اتاق 🚪🛏️</t>
   </si>
   <si>
     <t>room_rent_t2</t>
-  </si>
-  <si>
-    <t>📍 از بین شهرهای زیر یکی رو انتخاب کنید یا نام آن را وارد نمایید:</t>
   </si>
   <si>
     <t>room_rent_user_preview</t>
@@ -1334,7 +1297,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_اتاق✅️️️️💠
+    <t>💠✅️️️️ #اجاره_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1355,7 +1318,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_اتاق✅️️️️💠
+    <t>💠✅️️️️ #اجاره_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1377,7 +1340,7 @@
 Contact the [advertiser]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_اتاق✅️️️️💠
+    <t>💠✅️️️️ #اجاره_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1402,7 +1365,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره_اتاق✅️️️️💠
+    <t>💠✅️️️️ #اجاره_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1423,7 +1386,7 @@
     <t>room applicant</t>
   </si>
   <si>
-    <t>متقاضی اتاق🏠</t>
+    <t>متقاضی اتاق 🚪🛏️</t>
   </si>
   <si>
     <t>room_applicant_t1</t>
@@ -1432,7 +1395,7 @@
     <t>category: room applicant</t>
   </si>
   <si>
-    <t>📦 دسته بندی : متقاضی اتاق</t>
+    <t>📁 دسته بندی: متقاضی اتاق 🚪🛏️</t>
   </si>
   <si>
     <t>room_applicant_t2</t>
@@ -1449,7 +1412,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره اتاق ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1458,6 +1421,14 @@
   </si>
   <si>
     <t>room_applicant_user_view_ad</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ #متقاضی_اتاق ✅️️️️💠
+📍مربوط به شهر:  #[city]
+🔎 محدوده: [sub_city]
+🗓️️ تاریخ: از [start_date] تا [end_date]
+📝 نوع قرارداد: #[contract_status]
+[description]</t>
   </si>
   <si>
     <t>room_applicant_admin_preview</t>
@@ -1472,7 +1443,7 @@
 Contact the [advertiser]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره اتاق ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1495,7 +1466,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #اجاره اتاق ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_اتاق ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1512,7 +1483,7 @@
     <t>meldezettel</t>
   </si>
   <si>
-    <t>ملد هوایی📮</t>
+    <t>ملد هوایی 📭</t>
   </si>
   <si>
     <t>meldezettel_t1</t>
@@ -1521,7 +1492,7 @@
     <t>category: meldezettel</t>
   </si>
   <si>
-    <t>📦 دسته بندی : ملد هوایی📮</t>
+    <t>📁 دسته بندی: ملد هوایی 📭</t>
   </si>
   <si>
     <t>meldezettel_t2</t>
@@ -1539,7 +1510,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #meldezettel ✅️️️️💠
+    <t>💠✅️️️️ #ملد_هوایی ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1549,6 +1520,15 @@
   </si>
   <si>
     <t>meldezettel_user_view_ad</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ #ملد_هوایی ✅️️️️💠
+📍مربوط به شهر:  #[city]
+🔎 محدوده: [sub_city]
+🗓️️ تاریخ: از [start_date] تا [end_date]
+📝 نوع قرارداد: #[contract_status]
+[price_line]
+[description]</t>
   </si>
   <si>
     <t>meldezettel_admin_preview</t>
@@ -1566,7 +1546,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #meldezettel ✅️️️️💠
+    <t>💠✅️️️️ #ملد_هوایی ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1579,7 +1559,7 @@
     <t>meldezettel_channel_message</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #meldezettel ✅️️️️💠
+    <t>💠✅️️️️ #ملد_هوایی ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1597,7 +1577,7 @@
     <t>meldezettel applicant</t>
   </si>
   <si>
-    <t>متقاضی ملد هوایی📮</t>
+    <t>متقاضی ملد هوایی 📭</t>
   </si>
   <si>
     <t>meldezettel_applicant_t1</t>
@@ -1606,7 +1586,7 @@
     <t>category: meldezettel applicant</t>
   </si>
   <si>
-    <t>📦 دسته بندی : متقاضی ملد هوایی📮</t>
+    <t>📁 دسته بندی: متقاضی ملد هوایی 📭</t>
   </si>
   <si>
     <t>meldezettel_applicant_t2</t>
@@ -1622,7 +1602,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #meldezettel_applicant ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_ملد_هوایی ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1630,6 +1610,13 @@
   </si>
   <si>
     <t>meldezettel_applicant_user_view_ad</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ #متقاضی_ملد_هوایی ✅️️️️💠
+📍مربوط به شهر:  #[city]
+🔎 محدوده: [sub_city]
+🗓️️ تاریخ: از [start_date] تا [end_date]
+[description]</t>
   </si>
   <si>
     <t>meldezettel_applicant_admin_preview</t>
@@ -1645,7 +1632,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #meldezettel_applicant ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_ملد_هوایی ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1656,7 +1643,7 @@
     <t>meldezettel_applicant_channel_message</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #meldezettel_applicant ✅️️️️💠
+    <t>💠✅️️️️ #متقاضی_ملد_هوایی ✅️️️️💠
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
 🗓️️ تاریخ: از [start_date] تا [end_date]
@@ -1672,7 +1659,7 @@
     <t>selling goods</t>
   </si>
   <si>
-    <t>فروش کالا📦</t>
+    <t>فروش کالا 🛍️</t>
   </si>
   <si>
     <t>selling_goods_t1</t>
@@ -1681,7 +1668,7 @@
     <t>category: selling goods</t>
   </si>
   <si>
-    <t>📦 دسته بندی : فروش کالا📦</t>
+    <t>📁 دسته بندی: فروش کالا 🛍️</t>
   </si>
   <si>
     <t>selling_goods_t2</t>
@@ -1698,7 +1685,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #selling_goods ✅️️️️💠
+    <t>💠✅️️️️ فروش_کالا# ✅️️️️💠
 Product Name: [product_name]
 [price_line2]
 📍مربوط به شهر:  #[city]
@@ -1707,6 +1694,14 @@
   </si>
   <si>
     <t>selling_goods_user_view_ad</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ فروش_کالا# ✅️️️️💠
+Product Name: [product_name]
+[price_line2]
+📍مربوط به شهر:  #[city]
+🔎 محدوده: [sub_city]
+[description]</t>
   </si>
   <si>
     <t>selling_goods_admin_preview</t>
@@ -1723,7 +1718,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #selling_goods ✅️️️️💠
+    <t>💠✅️️️️ فروش_کالا# ✅️️️️💠
 Product Name: [product_name]
 [price_line2]
 📍مربوط به شهر:  #[city]
@@ -1735,7 +1730,7 @@
     <t>selling_goods_channel_message</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #selling_goods ✅️️️️💠
+    <t>💠✅️️️️ فروش_کالا# ✅️️️️💠
 Product Name: [product_name]
 [price_line2]
 📍مربوط به شهر:  #[city]
@@ -1752,7 +1747,7 @@
     <t>buying goods</t>
   </si>
   <si>
-    <t>خرید کالا📦</t>
+    <t>خرید کالا 🛍️</t>
   </si>
   <si>
     <t>buying_goods_t1</t>
@@ -1761,7 +1756,7 @@
     <t>category: buying goods</t>
   </si>
   <si>
-    <t>📦 دسته بندی : خرید کالا📦</t>
+    <t>📁 دسته بندی: خرید کالا 🛍️</t>
   </si>
   <si>
     <t>buying_goods_t2</t>
@@ -1777,7 +1772,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #buying_goods ✅️️️️💠
+    <t>💠✅️️️️ خرید_کالا# ✅️️️️💠
 Product Name: [product_name]
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
@@ -1794,7 +1789,7 @@
 [description]</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #buying_goods ✅️️️️💠
+    <t>💠✅️️️️ خرید_کالا# ✅️️️️💠
 Product Name: [product_name]
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
@@ -1814,7 +1809,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #buying_goods ✅️️️️💠
+    <t>💠✅️️️️ خرید_کالا# ✅️️️️💠
 Product Name: [product_name]
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
@@ -1835,7 +1830,7 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
-    <t>💠 ✅️️️️ #buying_goods ✅️️️️💠
+    <t>💠✅️️️️ خرید_کالا# ✅️️️️💠
 Product Name: [product_name]
 📍مربوط به شهر:  #[city]
 🔎 محدوده: [sub_city]
@@ -1851,7 +1846,7 @@
     <t>buying Cargo</t>
   </si>
   <si>
-    <t>فروش بار 📦</t>
+    <t>خرید بار 📦</t>
   </si>
   <si>
     <t>buying_cargo_t1</t>
@@ -1860,7 +1855,7 @@
     <t>category: buying Cargo</t>
   </si>
   <si>
-    <t>📦 دسته بندی : فروش بار📦</t>
+    <t>📁 دسته بندی: خرید بار 📦</t>
   </si>
   <si>
     <t>buying_cargo_t2</t>
@@ -1984,13 +1979,44 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ خرید_بار# ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]</t>
+  </si>
+  <si>
     <t>buying_cargo_user_view_ad</t>
   </si>
   <si>
+    <t>💠✅️️️️ خرید_بار# ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]</t>
+  </si>
+  <si>
     <t>buying_cargo_admin_preview</t>
   </si>
   <si>
     <t>💠 ✅️️️️ #buying_cargo ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ خرید_بار# ✅️️️️💠
 🚌 Origin and destination: #[from_to_city]
 Flight Date: [start_date]
 City of origin: [city]
@@ -2017,13 +2043,26 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
+    <t>💠✅️️️️ خرید_بار# ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
+  <si>
     <t>selling_cargo_btn</t>
   </si>
   <si>
     <t>selling Cargo</t>
   </si>
   <si>
-    <t>خرید بار 📦</t>
+    <t>فروش بار 📦</t>
   </si>
   <si>
     <t>selling_cargo_t1</t>
@@ -2032,7 +2071,7 @@
     <t>category: selling Cargo</t>
   </si>
   <si>
-    <t>📦 دسته بندی : خرید بار📦</t>
+    <t>📁 دسته بندی: فروش بار 📦</t>
   </si>
   <si>
     <t>selling_cargo_t2</t>
@@ -2102,13 +2141,44 @@
 [description]</t>
   </si>
   <si>
+    <t>💠 ✅️️️️ فروش_بار# ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]</t>
+  </si>
+  <si>
     <t>selling_cargo_user_view_ad</t>
   </si>
   <si>
+    <t>💠 ✅️️️️ فروش_بار# ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]</t>
+  </si>
+  <si>
     <t>selling_cargo_admin_preview</t>
   </si>
   <si>
     <t>💠 ✅️️️️ #selling_cargo ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>💠 ✅️️️️ فروش_بار# ✅️️️️💠
 🚌 Origin and destination: #[from_to_city]
 Flight Date: [start_date]
 City of origin: [city]
@@ -2135,16 +2205,35 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
+    <t>💠 ✅️️️️ فروش_بار# ✅️️️️💠
+🚌 Origin and destination: #[from_to_city]
+Flight Date: [start_date]
+City of origin: [city]
+Destination city: [city2]
+Load wight: [load]
+price per kilo: [price]
+[description]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
+  <si>
     <t>needs_btn</t>
   </si>
   <si>
     <t>needs</t>
   </si>
   <si>
+    <t>نیازمندی ها 🤝</t>
+  </si>
+  <si>
     <t>needs_t1</t>
   </si>
   <si>
     <t>category: needs</t>
+  </si>
+  <si>
+    <t>📁 دسته بندی: نیازمندی ها 🤝</t>
   </si>
   <si>
     <t>needs_t2</t>
@@ -2162,6 +2251,12 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ نیازمندی_ها# ✅️️️️💠
+City: [city]
+[price_line]
+[description]</t>
+  </si>
+  <si>
     <t>needs_user_view_ad</t>
   </si>
   <si>
@@ -2171,10 +2266,23 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ نیازمندی_ها# ✅️️️️💠
+City: [city]
+[price_line]
+[description]</t>
+  </si>
+  <si>
     <t>needs_admin_preview</t>
   </si>
   <si>
     <t>💠 ✅️️️️ #needs✅️️️️💠
+City: [city]
+[price_line]
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ نیازمندی_ها# ✅️️️️💠
 City: [city]
 [price_line]
 [description]
@@ -2193,16 +2301,31 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
+    <t>💠✅️️️️ نیازمندی_ها# ✅️️️️💠
+City: [city]
+[price_line]
+[description]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
+  <si>
     <t>buying_euro_btn</t>
   </si>
   <si>
     <t>euro buy</t>
   </si>
   <si>
+    <t>خرید یورو 💶</t>
+  </si>
+  <si>
     <t>buying_euro_t1</t>
   </si>
   <si>
     <t>category: euro buy</t>
+  </si>
+  <si>
+    <t>📁 دسته بندی: خرید یورو 💶</t>
   </si>
   <si>
     <t>buying_euro_t2</t>
@@ -2305,6 +2428,13 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ خرید_یورو# ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]</t>
+  </si>
+  <si>
     <t>buying_euro_user_view_ad</t>
   </si>
   <si>
@@ -2315,10 +2445,25 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ خرید_یورو# ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]</t>
+  </si>
+  <si>
     <t>buying_euro_admin_preview</t>
   </si>
   <si>
     <t>💠 ✅️️️️ #buying_euro ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ خرید_یورو# ✅️️️️💠
 Euros: [euros]
 pricing: [toman_per_euro]
 Payment methods: [payment_methods]
@@ -2339,16 +2484,32 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
+    <t>💠✅️️️️ خرید_یورو# ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
+  <si>
     <t>selling_euro_btn</t>
   </si>
   <si>
     <t>euro sell</t>
   </si>
   <si>
+    <t>فروش یورو 💶</t>
+  </si>
+  <si>
     <t>selling_euro_t1</t>
   </si>
   <si>
     <t>category: euro sell</t>
+  </si>
+  <si>
+    <t>📁 دسته بندی: فروش یورو 💶</t>
   </si>
   <si>
     <t>selling_euro_t2</t>
@@ -2376,20 +2537,35 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ فروش_یورو# ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]</t>
+  </si>
+  <si>
+    <t>selling_euro_user_view_ad</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ فروش_یورو# ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]</t>
+  </si>
+  <si>
+    <t>selling_euro_admin_preview</t>
+  </si>
+  <si>
     <t>💠 ✅️️️️ #selling_euro ✅️️️️💠
 Euros: [euros]
 pricing: [toman_per_euro]
 Payment methods: [payment_methods]
-[description]</t>
-  </si>
-  <si>
-    <t>selling_euro_user_view_ad</t>
-  </si>
-  <si>
-    <t>selling_euro_admin_preview</t>
-  </si>
-  <si>
-    <t>💠 ✅️️️️ #selling_euro ✅️️️️💠
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ فروش_یورو# ✅️️️️💠
 Euros: [euros]
 pricing: [toman_per_euro]
 Payment methods: [payment_methods]
@@ -2410,16 +2586,32 @@
 ✅️️️️️️️ @channel_username</t>
   </si>
   <si>
+    <t>💠✅️️️️ فروش_یورو# ✅️️️️💠
+Euros: [euros]
+pricing: [toman_per_euro]
+Payment methods: [payment_methods]
+[description]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
+  <si>
     <t>services_btn</t>
   </si>
   <si>
     <t>services</t>
   </si>
   <si>
+    <t>خدمات 🤝</t>
+  </si>
+  <si>
     <t>services_t1</t>
   </si>
   <si>
     <t>category: services</t>
+  </si>
+  <si>
+    <t>📁 دسته بندی: خدمات 🤝</t>
   </si>
   <si>
     <t>services_t2</t>
@@ -2440,25 +2632,32 @@
 [description]</t>
   </si>
   <si>
+    <t>💠✅️️️️ خدمات# ✅️️️️💠
+Service: [service_name]
+City: [city]
+[description]</t>
+  </si>
+  <si>
+    <t>services_user_view_ad</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ خدمات# ✅️️️️💠
+Service: [service_name]
+City: [city]
+[description]</t>
+  </si>
+  <si>
+    <t>services_admin_preview</t>
+  </si>
+  <si>
     <t>💠 ✅️️️️ #services✅️️️️💠
 Service: [service_name]
 City: [city]
-[description]</t>
-  </si>
-  <si>
-    <t>services_user_view_ad</t>
-  </si>
-  <si>
-    <t>💠 ✅️️️️ #services✅️️️️💠
-Service: [service_name]
-City: [city]
-[description]</t>
-  </si>
-  <si>
-    <t>services_admin_preview</t>
-  </si>
-  <si>
-    <t>💠 ✅️️️️ #services✅️️️️💠
+[description]
+Contact the [advertiser]</t>
+  </si>
+  <si>
+    <t>💠✅️️️️ خدمات# ✅️️️️💠
 Service: [service_name]
 City: [city]
 [description]
@@ -2476,12 +2675,21 @@
 🤖️️️ @bot_username
 ✅️️️️️️️ @channel_username</t>
   </si>
+  <si>
+    <t>💠✅️️️️ خدمات# ✅️️️️💠
+Service: [service_name]
+City: [city]
+[description]
+Contact the [advertiser]
+🤖️️️ @bot_username
+✅️️️️️️️ @channel_username</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2502,12 +2710,6 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12.0"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -2579,13 +2781,13 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2594,10 +2796,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -4283,35 +4485,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -4321,46 +4523,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>416</v>
-      </c>
       <c r="C9" s="11" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -4601,35 +4803,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -4639,46 +4841,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>429</v>
+      <c r="C7" s="19" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>433</v>
+        <v>435</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>432</v>
-      </c>
-      <c r="C9" s="7" t="s">
         <v>435</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -4914,35 +5116,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -4952,46 +5154,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>445</v>
+        <v>447</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>448</v>
+        <v>450</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>451</v>
+        <v>453</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>453</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>454</v>
+        <v>456</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -5227,13 +5429,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -5243,24 +5445,24 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
@@ -5270,24 +5472,24 @@
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
@@ -5297,24 +5499,24 @@
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
@@ -5324,24 +5526,24 @@
     </row>
     <row r="13" ht="21.0" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
@@ -5351,24 +5553,24 @@
     </row>
     <row r="16" ht="21.0" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" ht="21.0" customHeight="1">
@@ -5378,24 +5580,24 @@
     </row>
     <row r="19" ht="21.0" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" ht="21.0" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
@@ -5405,35 +5607,35 @@
     </row>
     <row r="22" ht="21.0" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="23" ht="21.0" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="24" ht="21.0" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="25" ht="21.0" customHeight="1">
@@ -5443,46 +5645,46 @@
     </row>
     <row r="26" ht="21.0" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" ht="21.0" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="29" ht="21.0" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" ht="21.0" customHeight="1">
@@ -5492,46 +5694,46 @@
     </row>
     <row r="31" ht="21.0" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
     </row>
     <row r="32" ht="21.0" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
     <row r="33" ht="21.0" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
     </row>
     <row r="34" ht="21.0" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
     </row>
     <row r="35" ht="21.0" customHeight="1">
@@ -5607,13 +5809,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -5623,24 +5825,24 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
@@ -5650,24 +5852,24 @@
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
@@ -5677,24 +5879,24 @@
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
@@ -5704,24 +5906,24 @@
     </row>
     <row r="13" ht="21.0" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
@@ -5731,24 +5933,24 @@
     </row>
     <row r="16" ht="21.0" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" ht="21.0" customHeight="1">
@@ -5758,24 +5960,24 @@
     </row>
     <row r="19" ht="21.0" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" ht="21.0" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
@@ -5785,35 +5987,35 @@
     </row>
     <row r="22" ht="21.0" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="23" ht="21.0" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="24" ht="21.0" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="25" ht="21.0" customHeight="1">
@@ -5823,46 +6025,46 @@
     </row>
     <row r="26" ht="21.0" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" ht="21.0" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="29" ht="21.0" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" ht="21.0" customHeight="1">
@@ -5872,46 +6074,46 @@
     </row>
     <row r="31" ht="21.0" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="32" ht="21.0" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
     </row>
     <row r="33" ht="21.0" customHeight="1">
       <c r="A33" s="7" t="s">
-        <v>531</v>
+        <v>540</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>532</v>
+        <v>541</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>532</v>
+        <v>542</v>
       </c>
     </row>
     <row r="34" ht="21.0" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>533</v>
+        <v>543</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>534</v>
+        <v>545</v>
       </c>
     </row>
     <row r="35" ht="21.0" customHeight="1">
@@ -5987,13 +6189,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>535</v>
+        <v>546</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>536</v>
+        <v>547</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -6003,24 +6205,24 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>537</v>
+        <v>549</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>538</v>
+        <v>550</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>539</v>
+        <v>552</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
@@ -6035,46 +6237,46 @@
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>541</v>
+        <v>554</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>542</v>
+        <v>555</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>542</v>
+        <v>556</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>543</v>
+        <v>557</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>544</v>
+        <v>558</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>544</v>
+        <v>559</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>545</v>
+        <v>560</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>546</v>
+        <v>561</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>546</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>547</v>
+        <v>563</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>548</v>
+        <v>564</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>548</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -6115,13 +6317,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>549</v>
+        <v>566</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>550</v>
+        <v>567</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -6131,24 +6333,24 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>552</v>
+        <v>570</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>553</v>
+        <v>572</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>554</v>
+        <v>573</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>554</v>
+        <v>573</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
@@ -6163,46 +6365,46 @@
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>555</v>
+        <v>574</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>556</v>
+        <v>575</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>556</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>557</v>
+        <v>576</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>558</v>
+        <v>577</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>558</v>
+        <v>577</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>559</v>
+        <v>578</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>560</v>
+        <v>579</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>560</v>
+        <v>579</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>561</v>
+        <v>580</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>562</v>
+        <v>581</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>562</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
@@ -6212,106 +6414,106 @@
     </row>
     <row r="13" ht="21.0" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>563</v>
+        <v>582</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>564</v>
+        <v>583</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>565</v>
+        <v>584</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>566</v>
+        <v>585</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>567</v>
+        <v>586</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>567</v>
+        <v>586</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>568</v>
+        <v>587</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>569</v>
+        <v>588</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>569</v>
+        <v>588</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>570</v>
+        <v>589</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>571</v>
+        <v>590</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>571</v>
+        <v>590</v>
       </c>
     </row>
     <row r="17" ht="21.0" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>572</v>
+        <v>591</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>573</v>
+        <v>592</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>573</v>
+        <v>592</v>
       </c>
     </row>
     <row r="18" ht="21.0" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>574</v>
+        <v>593</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>575</v>
+        <v>594</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>575</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" ht="21.0" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>576</v>
+        <v>595</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>577</v>
+        <v>596</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>577</v>
+        <v>596</v>
       </c>
     </row>
     <row r="20" ht="21.0" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>578</v>
+        <v>597</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>579</v>
+        <v>598</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>579</v>
+        <v>598</v>
       </c>
     </row>
     <row r="21" ht="21.0" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>580</v>
+        <v>599</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>581</v>
+        <v>600</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>581</v>
+        <v>600</v>
       </c>
     </row>
     <row r="22" ht="21.0" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>245</v>
@@ -6327,46 +6529,46 @@
     </row>
     <row r="24" ht="21.0" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>583</v>
+        <v>602</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>584</v>
+        <v>603</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>584</v>
+        <v>604</v>
       </c>
     </row>
     <row r="25" ht="21.0" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>586</v>
+        <v>606</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>586</v>
+        <v>607</v>
       </c>
     </row>
     <row r="26" ht="21.0" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>587</v>
+        <v>608</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>588</v>
+        <v>609</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>588</v>
+        <v>610</v>
       </c>
     </row>
     <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="7" t="s">
-        <v>589</v>
+        <v>611</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>590</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -6407,13 +6609,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>591</v>
+        <v>614</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>592</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>592</v>
+        <v>615</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -6423,24 +6625,24 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>593</v>
+        <v>617</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>594</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>594</v>
+        <v>618</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>595</v>
+        <v>620</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>596</v>
+        <v>621</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>596</v>
+        <v>621</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
@@ -6450,24 +6652,24 @@
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>597</v>
+        <v>622</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>598</v>
+        <v>623</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>598</v>
+        <v>623</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>599</v>
+        <v>624</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>564</v>
+        <v>583</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>565</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
@@ -6477,46 +6679,46 @@
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>600</v>
+        <v>625</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>601</v>
+        <v>626</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>602</v>
+        <v>627</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>603</v>
+        <v>628</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>601</v>
+        <v>626</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>602</v>
+        <v>629</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>604</v>
+        <v>630</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>605</v>
+        <v>631</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>605</v>
+        <v>632</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>606</v>
+        <v>633</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>607</v>
+        <v>634</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>607</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -6557,13 +6759,13 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>608</v>
+        <v>636</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>609</v>
+        <v>637</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
@@ -6573,35 +6775,35 @@
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>610</v>
+        <v>639</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>611</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>611</v>
+        <v>640</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>612</v>
+        <v>642</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>613</v>
+        <v>643</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>614</v>
+        <v>644</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>614</v>
+        <v>644</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
@@ -6611,46 +6813,46 @@
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>615</v>
+        <v>645</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>616</v>
+        <v>646</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>617</v>
+        <v>647</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>618</v>
+        <v>648</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>616</v>
+        <v>646</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>619</v>
+        <v>649</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>620</v>
+        <v>650</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>621</v>
+        <v>651</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>621</v>
+        <v>652</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>622</v>
+        <v>653</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>623</v>
+        <v>654</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>623</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -13123,14 +13325,10 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="C11"/>
-    <hyperlink r:id="rId2" ref="C12"/>
-  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14763,7 +14961,7 @@
         <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -14773,46 +14971,46 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>359</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="11" t="s">
         <v>365</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>368</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">
@@ -15013,7 +15211,7 @@
     </row>
     <row r="48" ht="21.0" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>299</v>
@@ -15087,35 +15285,35 @@
     </row>
     <row r="2" ht="21.0" customHeight="1">
       <c r="A2" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>372</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
       <c r="A3" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>375</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -15125,24 +15323,24 @@
     </row>
     <row r="6" ht="21.0" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>379</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>381</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
@@ -15433,7 +15631,7 @@
         <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>357</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="1">
@@ -15460,29 +15658,29 @@
         <v>396</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="1">

</xml_diff>